<commit_message>
adding the files to git
</commit_message>
<xml_diff>
--- a/sapp/static/docs/projectDetails.xlsx
+++ b/sapp/static/docs/projectDetails.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ish\OneDrive - Carleton University\work details\Projects\Self assessment 4th year project\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ish\Desktop\current project\selfassessment\sapp\static\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_990AAE22D25631ED5E38DBBD46CC2A17CC548F29" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{98223731-BD66-438A-B32F-A2D868898007}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A99CFDB-B65E-4F51-8171-412DF171931A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="405" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project List" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Labiche</t>
   </si>
@@ -33,30 +33,6 @@
     <t>Singh</t>
   </si>
   <si>
-    <t>First name</t>
-  </si>
-  <si>
-    <t>Last name</t>
-  </si>
-  <si>
-    <t>ID Number</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Student</t>
-  </si>
-  <si>
-    <t>Co-supervisor</t>
-  </si>
-  <si>
-    <t>Supervisor</t>
-  </si>
-  <si>
-    <t>Group</t>
-  </si>
-  <si>
     <t>Crowd-source grocery store layouts for dynamically sorted shopping lists</t>
   </si>
   <si>
@@ -93,7 +69,28 @@
     <t>Ishdeep</t>
   </si>
   <si>
-    <t>Group No</t>
+    <t>assessmentStatus</t>
+  </si>
+  <si>
+    <t>groupNo</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>supervisor</t>
+  </si>
+  <si>
+    <t>coSupervisor</t>
+  </si>
+  <si>
+    <t>userId</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>firstName</t>
   </si>
 </sst>
 </file>
@@ -238,23 +235,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -535,7 +530,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
@@ -553,154 +548,155 @@
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="13">
+        <v>52</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="14"/>
+      <c r="E2" s="9">
+        <v>1</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="9">
+        <v>2</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="1">
+        <v>3</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
+      <c r="G4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="10" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
+        <v>27</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="7">
+        <v>4</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="13"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="10">
         <v>5</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>2</v>
+      <c r="F6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
-        <v>52</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="9">
-        <v>1</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="9">
-        <v>2</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="1">
-        <v>3</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="15">
-        <v>27</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="7">
-        <v>4</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="12">
-        <v>5</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <mergeCells count="13">
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="D3:D5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
+  <mergeCells count="9">
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
   </mergeCells>
   <pageMargins left="0.1" right="0.1" top="0.1" bottom="0.1" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
adding the test data for office admin and changing the user uploader
</commit_message>
<xml_diff>
--- a/sapp/static/docs/projectDetails.xlsx
+++ b/sapp/static/docs/projectDetails.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cmailcarletonca-my.sharepoint.com/personal/ishdeepsingh_cmail_carleton_ca/Documents/work details/Projects/Self assessment 4th year project/resources/sample/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cmailcarletonca-my.sharepoint.com/personal/ishdeepsingh_cmail_carleton_ca/Documents/work details/Projects/Self assessment 4th year project/resources/testusersinfo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{1A99CFDB-B65E-4F51-8171-412DF171931A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D3BF814A-423F-4005-9CED-D3AA1EF301EE}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{1A99CFDB-B65E-4F51-8171-412DF171931A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{93455425-9B9B-4902-BBAF-A7FDC74B3843}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21210" windowHeight="12750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25545" yWindow="1905" windowWidth="21210" windowHeight="12750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project List" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>Labiche</t>
   </si>
@@ -33,12 +33,6 @@
     <t>Singh</t>
   </si>
   <si>
-    <t>Crowd-source grocery store layouts for dynamically sorted shopping lists</t>
-  </si>
-  <si>
-    <t>Green</t>
-  </si>
-  <si>
     <t>assessmentStatus</t>
   </si>
   <si>
@@ -81,23 +75,47 @@
     <t>Jennifer</t>
   </si>
   <si>
-    <t>Living the GA dream</t>
-  </si>
-  <si>
-    <t>Hebert</t>
-  </si>
-  <si>
-    <t>Darlene</t>
-  </si>
-  <si>
     <t>Ishdeep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Department of systema and computer engineering - admin staff </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Department of systema and computer engineering - Tech  staff </t>
+  </si>
+  <si>
+    <t>Buburuz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jerry </t>
+  </si>
+  <si>
+    <t>Russ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daren </t>
+  </si>
+  <si>
+    <t>Chiv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kong </t>
+  </si>
+  <si>
+    <t>East</t>
+  </si>
+  <si>
+    <t>Erica</t>
+  </si>
+  <si>
+    <t>Yvan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -105,6 +123,12 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
@@ -119,7 +143,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -150,19 +174,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -216,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFill="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -224,7 +235,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -232,15 +242,19 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -521,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,145 +553,217 @@
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="E1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="F1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="H1" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
         <v>10</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="B2" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="12"/>
+      <c r="E2" s="1">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="11"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="1">
         <v>11</v>
       </c>
-      <c r="H1" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="12">
-        <v>52</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="1">
-        <v>2</v>
-      </c>
-      <c r="F2" s="5" t="s">
+      <c r="F3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="11"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="1">
         <v>12</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="F4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="11"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="1">
         <v>13</v>
       </c>
-      <c r="H2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="1">
-        <v>3</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="F5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="1">
         <v>14</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
+        <v>20</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="8">
         <v>15</v>
       </c>
-      <c r="H3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="1">
-        <v>4</v>
-      </c>
-      <c r="F4" s="3" t="s">
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="14">
         <v>16</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="14">
         <v>17</v>
       </c>
-      <c r="H4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="12">
-        <v>27</v>
-      </c>
-      <c r="B5" s="13" t="s">
+      <c r="F9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="9">
         <v>18</v>
       </c>
-      <c r="C5" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="9">
-        <v>5</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="10">
-        <v>6</v>
-      </c>
-      <c r="F6" s="11" t="s">
+      <c r="F10" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G6" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" s="1">
+      <c r="G10" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="1">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="8">
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="D2:D6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:D10"/>
   </mergeCells>
   <pageMargins left="0.1" right="0.1" top="0.1" bottom="0.1" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>